<commit_message>
Added data transformation logic
</commit_message>
<xml_diff>
--- a/employees_db.xlsx
+++ b/employees_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Personal Projects\etl_pipeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\loni\etl_pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE9E3DC-DD3B-495F-9CAB-BEDD1306CFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B7D49F-3067-4725-8070-75C9A91F2B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9B12A498-3941-43C1-9C68-26DF91974B68}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{9B12A498-3941-43C1-9C68-26DF91974B68}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="137">
   <si>
     <t>ID</t>
   </si>
@@ -288,16 +288,183 @@
   </si>
   <si>
     <t>Emergency Contact ID</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>249-314-8464x78504</t>
+  </si>
+  <si>
+    <t>greenelisa@taylor.com</t>
+  </si>
+  <si>
+    <t>001-026-940-4742x421</t>
+  </si>
+  <si>
+    <t>estradaduane@gmail.com</t>
+  </si>
+  <si>
+    <t>483-425-8747x024</t>
+  </si>
+  <si>
+    <t>georgecharles@ibarra.net</t>
+  </si>
+  <si>
+    <t>(148)357-6809</t>
+  </si>
+  <si>
+    <t>montoyazachary@hotmail.com</t>
+  </si>
+  <si>
+    <t>+1-934-130-9265x7704</t>
+  </si>
+  <si>
+    <t>aliciamiles@hotmail.com</t>
+  </si>
+  <si>
+    <t>jason55@silva.org</t>
+  </si>
+  <si>
+    <t>755.065.7576</t>
+  </si>
+  <si>
+    <t>wtaylor@patterson.com</t>
+  </si>
+  <si>
+    <t>(220)947-2179x0882</t>
+  </si>
+  <si>
+    <t>ronald52@williams-diaz.com</t>
+  </si>
+  <si>
+    <t>(063)565-1128x34128</t>
+  </si>
+  <si>
+    <t>tashacoleman@wilson-arroyo.net</t>
+  </si>
+  <si>
+    <t>903-560-2517x617</t>
+  </si>
+  <si>
+    <t>andrew30@hotmail.com</t>
+  </si>
+  <si>
+    <t>001-507-985-1908</t>
+  </si>
+  <si>
+    <t>moorepamela@miller.com</t>
+  </si>
+  <si>
+    <t>(177)748-2382x16014</t>
+  </si>
+  <si>
+    <t>sheilawood@hotmail.com</t>
+  </si>
+  <si>
+    <t>625.599.6027x1810</t>
+  </si>
+  <si>
+    <t>william70@yahoo.com</t>
+  </si>
+  <si>
+    <t>001-883-960-3461x992</t>
+  </si>
+  <si>
+    <t>rodriguezdaniel@lozano.com</t>
+  </si>
+  <si>
+    <t>+1-554-063-3340x60624</t>
+  </si>
+  <si>
+    <t>anna62@small-cabrera.net</t>
+  </si>
+  <si>
+    <t>385-267-7200x6417</t>
+  </si>
+  <si>
+    <t>valerieturner@yahoo.com</t>
+  </si>
+  <si>
+    <t>344.777.1248</t>
+  </si>
+  <si>
+    <t>douglas23@gmail.com</t>
+  </si>
+  <si>
+    <t>371.766.5543x26145</t>
+  </si>
+  <si>
+    <t>james57@byrd-montgomery.info</t>
+  </si>
+  <si>
+    <t>001-679-833-4075x599</t>
+  </si>
+  <si>
+    <t>ihawkins@harris.com</t>
+  </si>
+  <si>
+    <t>404-934-4288x547</t>
+  </si>
+  <si>
+    <t>benjamin32@anderson.com</t>
+  </si>
+  <si>
+    <t>(196)702-2189x50882</t>
+  </si>
+  <si>
+    <t>bartondiana@hotmail.com</t>
+  </si>
+  <si>
+    <t>787.058.3313</t>
+  </si>
+  <si>
+    <t>taylor12@yahoo.com</t>
+  </si>
+  <si>
+    <t>(286)792-3780x568</t>
+  </si>
+  <si>
+    <t>laura40@hotmail.com</t>
+  </si>
+  <si>
+    <t>ericjones@hotmail.com</t>
+  </si>
+  <si>
+    <t>(071)556-2873x521</t>
+  </si>
+  <si>
+    <t>nsavage@yahoo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -320,10 +487,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -331,8 +499,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -665,24 +840,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5E2C2B-C213-48B3-A514-36B2D3262282}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="6.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="6" width="15.453125" customWidth="1"/>
-    <col min="7" max="9" width="14.26953125" customWidth="1"/>
-    <col min="10" max="10" width="27.7265625" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,28 +866,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -724,29 +906,38 @@
       <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="2">
         <v>35138</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="L2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="1">
         <v>1023</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -756,29 +947,38 @@
       <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" s="2">
         <v>35269</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="L3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3" s="1">
         <v>1024</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -788,29 +988,38 @@
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="2">
+      <c r="J4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" s="2">
         <v>35379</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="L4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="1">
         <v>1025</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -820,29 +1029,38 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="2">
         <v>35435</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="L5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="1">
         <v>1026</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -852,29 +1070,38 @@
       <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="2">
         <v>35567</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="L6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M6" s="1">
         <v>1027</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -884,29 +1111,38 @@
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3">
+        <v>667777777</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="2">
         <v>35703</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="L7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M7" s="1">
         <v>1028</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -916,29 +1152,38 @@
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="2">
+      <c r="J8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K8" s="2">
         <v>35854</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="L8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M8" s="1">
         <v>1029</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -948,29 +1193,38 @@
       <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9" s="2">
         <v>35958</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="L9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="1">
         <v>1030</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -980,29 +1234,38 @@
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="2">
         <v>36093</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="L10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="1">
         <v>1031</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1012,29 +1275,38 @@
       <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K11" s="2">
         <v>36253</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="L11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" s="1">
         <v>1032</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1044,29 +1316,38 @@
       <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K12" s="2">
         <v>36391</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J12" s="1">
+      <c r="L12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M12" s="1">
         <v>1033</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1076,29 +1357,38 @@
       <c r="C13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="2">
+      <c r="J13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="2">
         <v>36501</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="L13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" s="1">
         <v>1034</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -1108,29 +1398,38 @@
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="2">
-        <v>36607</v>
+      <c r="H14" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J14" s="1">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14" s="2">
+        <v>36093</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -1140,29 +1439,38 @@
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="2">
-        <v>36722</v>
+      <c r="H15" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J15" s="1">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="2">
+        <v>36253</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1172,29 +1480,38 @@
       <c r="C16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="2">
+      <c r="I16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K16" s="2">
         <v>36832</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="1">
+      <c r="M16" s="1">
         <v>1037</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1204,29 +1521,38 @@
       <c r="C17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" s="2">
+      <c r="I17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K17" s="2">
         <v>36909</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J17" s="1">
+      <c r="M17" s="1">
         <v>1038</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1236,29 +1562,38 @@
       <c r="C18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K18" s="2">
         <v>37041</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J18" s="1">
+      <c r="L18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M18" s="1">
         <v>1039</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1268,29 +1603,38 @@
       <c r="C19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" s="2">
+      <c r="I19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K19" s="2">
         <v>37148</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J19" s="1">
+      <c r="M19" s="1">
         <v>1040</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1300,29 +1644,38 @@
       <c r="C20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="2">
+      <c r="J20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K20" s="2">
         <v>37292</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J20" s="1">
+      <c r="M20" s="1">
         <v>1041</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1332,29 +1685,38 @@
       <c r="C21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H21" s="2">
+      <c r="I21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K21" s="2">
         <v>37434</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="1">
+      <c r="M21" s="1">
         <v>1042</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1364,29 +1726,38 @@
       <c r="C22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="2">
+      <c r="I22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K22" s="2">
         <v>37540</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J22" s="1">
+      <c r="M22" s="1">
         <v>1043</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1396,29 +1767,38 @@
       <c r="C23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="2">
+      <c r="J23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K23" s="2">
         <v>37689</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J23" s="1">
+      <c r="L23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M23" s="1">
         <v>1044</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1428,29 +1808,38 @@
       <c r="C24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K24" s="2">
         <v>37822</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J24" s="1">
+      <c r="L24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M24" s="1">
         <v>1045</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1460,29 +1849,38 @@
       <c r="C25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" s="2">
+      <c r="I25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K25" s="2">
         <v>37943</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J25" s="1">
+      <c r="M25" s="1">
         <v>1046</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1492,29 +1890,38 @@
       <c r="C26" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H26" s="2">
+      <c r="J26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K26" s="2">
         <v>38091</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J26" s="1">
+      <c r="M26" s="1">
         <v>1047</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1524,29 +1931,38 @@
       <c r="C27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="3">
+        <v>7921855040</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" s="2">
+      <c r="H27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K27" s="2">
         <v>38229</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J27" s="1">
+      <c r="L27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M27" s="1">
         <v>1048</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1556,29 +1972,38 @@
       <c r="C28" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="2">
+      <c r="J28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K28" s="2">
         <v>38707</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J28" s="1">
+      <c r="L28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M28" s="1">
         <v>1049</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>23</v>
       </c>
@@ -1588,29 +2013,38 @@
       <c r="C29" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H29" s="2">
+      <c r="H29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K29" s="2">
         <v>37822</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" s="1">
+      <c r="L29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M29" s="1">
         <v>1045</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>24</v>
       </c>
@@ -1620,29 +2054,45 @@
       <c r="C30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" s="2">
+      <c r="I30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K30" s="2">
         <v>37943</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J30" s="1">
+      <c r="M30" s="1">
         <v>1046</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E16" r:id="rId1" display="mailto:william70@yahoo.com" xr:uid="{318A2CE1-0549-4EF0-942E-F7ECB146A2C2}"/>
+    <hyperlink ref="E19" r:id="rId2" display="mailto:valerieturner@yahoo.com" xr:uid="{98A4DB25-E202-4148-9E9A-EBE7FE298FCB}"/>
+    <hyperlink ref="E25" r:id="rId3" display="mailto:taylor12@yahoo.com" xr:uid="{206D660A-7E10-4FC0-A810-80A171B86723}"/>
+    <hyperlink ref="E28" r:id="rId4" display="mailto:nsavage@yahoo.com" xr:uid="{345097A9-92F6-469E-881A-958F46EFF64F}"/>
+    <hyperlink ref="E30" r:id="rId5" display="mailto:taylor12@yahoo.com" xr:uid="{92F633DE-41B5-401D-9FA3-133069D18A82}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>